<commit_message>
added visualisations and things
</commit_message>
<xml_diff>
--- a/documents/data description.xlsx
+++ b/documents/data description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthurlanglois/Dropbox/My Mac (Arthur’s MacBook Pro)/Desktop/Spring 2022/Math Seminar/capstone/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74867D75-EF65-9B42-BDEC-E1A3DBACA398}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3366AF42-C333-D944-9117-B40651F7B02B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E25AC7C5-D538-F44E-9E78-A31A7B7C7BF5}"/>
+    <workbookView xWindow="2140" yWindow="1400" windowWidth="28800" windowHeight="16480" xr2:uid="{E25AC7C5-D538-F44E-9E78-A31A7B7C7BF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Variable</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>World Health Organization</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Age</t>
   </si>
 </sst>
 </file>
@@ -528,7 +540,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A3" sqref="A3:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="57.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,14 +737,26 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>